<commit_message>
added verified_relations excel sheet
</commit_message>
<xml_diff>
--- a/Schema_design_excel_sheet.xlsx
+++ b/Schema_design_excel_sheet.xlsx
@@ -8,31 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sunbeam_KDAC\Project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0957237F-33EF-40AD-B8B9-9F866BCD72AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B31863A-EBC0-47BF-BF6B-259E5C1EC08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER MANAGEMENT MODULE" sheetId="1" r:id="rId1"/>
     <sheet name="DRIVER MANAGEMENT MODULE" sheetId="13" r:id="rId2"/>
-    <sheet name="AUTHENTICATION &amp; SECURITY MODUL" sheetId="2" r:id="rId3"/>
-    <sheet name="ADDRESS MANAGEMENT MODULE" sheetId="3" r:id="rId4"/>
-    <sheet name="VEHICLE MANAGEMENT MODULE" sheetId="4" r:id="rId5"/>
-    <sheet name="SERVICE &amp; QUOTATION MODULE" sheetId="5" r:id="rId6"/>
-    <sheet name="BOOKING &amp; GOODS MGMT. MODULE" sheetId="6" r:id="rId7"/>
-    <sheet name="PAYMENT &amp; REWARDS MODULE" sheetId="7" r:id="rId8"/>
-    <sheet name="TRACKING &amp; DELIVERY MODULE" sheetId="8" r:id="rId9"/>
-    <sheet name="COMMUNICATION &amp; NOTIFICATION" sheetId="9" r:id="rId10"/>
-    <sheet name="DOCUMENTS &amp; VERIFICATION MODULE" sheetId="10" r:id="rId11"/>
-    <sheet name="BRANCH MANAGEMENT MODULE" sheetId="11" r:id="rId12"/>
-    <sheet name="ADMIN CONTROL MODULE" sheetId="12" r:id="rId13"/>
+    <sheet name="EMPLOYEE MANAGEMENT MODULE" sheetId="14" r:id="rId3"/>
+    <sheet name="AUTHENTICATION &amp; SECURITY MODUL" sheetId="2" r:id="rId4"/>
+    <sheet name="ADDRESS MANAGEMENT MODULE" sheetId="3" r:id="rId5"/>
+    <sheet name="VEHICLE MANAGEMENT MODULE" sheetId="4" r:id="rId6"/>
+    <sheet name="SERVICE &amp; QUOTATION MODULE" sheetId="5" r:id="rId7"/>
+    <sheet name="BOOKING &amp; GOODS MGMT. MODULE" sheetId="6" r:id="rId8"/>
+    <sheet name="PAYMENT &amp; REWARDS MODULE" sheetId="7" r:id="rId9"/>
+    <sheet name="TRACKING &amp; DELIVERY MODULE" sheetId="8" r:id="rId10"/>
+    <sheet name="COMMUNICATION &amp; NOTIFICATION" sheetId="9" r:id="rId11"/>
+    <sheet name="DOCUMENTS &amp; VERIFICATION MODULE" sheetId="10" r:id="rId12"/>
+    <sheet name="BRANCH MANAGEMENT MODULE" sheetId="11" r:id="rId13"/>
+    <sheet name="ADMIN CONTROL MODULE" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="495">
   <si>
     <t>Attribute</t>
   </si>
@@ -1406,6 +1407,117 @@
   </si>
   <si>
     <t>Type(s) of vehicle the driver can operate</t>
+  </si>
+  <si>
+    <t>EMPLOYEE</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>employee_id (PK)</t>
+  </si>
+  <si>
+    <t>Unique employee ID</t>
+  </si>
+  <si>
+    <t>Employee’s first name</t>
+  </si>
+  <si>
+    <t>Employee’s last name</t>
+  </si>
+  <si>
+    <t>Unique email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>hire_date</t>
+  </si>
+  <si>
+    <t>Date of joining</t>
+  </si>
+  <si>
+    <t>Employment status</t>
+  </si>
+  <si>
+    <t>role_id (FK)</t>
+  </si>
+  <si>
+    <t>Links to role table (optional)</t>
+  </si>
+  <si>
+    <t>user_id (FK)</t>
+  </si>
+  <si>
+    <t>Links to user account for login (optional)</t>
+  </si>
+  <si>
+    <t>EMPLYEE_ASSIGNMENT</t>
+  </si>
+  <si>
+    <t>assignment_id (PK)</t>
+  </si>
+  <si>
+    <t>employee_id (FK)</t>
+  </si>
+  <si>
+    <t>Assigned employee</t>
+  </si>
+  <si>
+    <t>customer_request_id (FK)</t>
+  </si>
+  <si>
+    <t>The customer’s relocation request</t>
+  </si>
+  <si>
+    <t>assigned_date</t>
+  </si>
+  <si>
+    <t>When assigned</t>
+  </si>
+  <si>
+    <t>ENUM('pending','in-progress','completed')</t>
+  </si>
+  <si>
+    <t>EMPLOYEE_PAYMENT</t>
+  </si>
+  <si>
+    <t>payment_id (PK)</t>
+  </si>
+  <si>
+    <t>Employee reference</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>Amount paid or handled</t>
+  </si>
+  <si>
+    <t>payment_type</t>
+  </si>
+  <si>
+    <t>ENUM('salary','commission','bonus')</t>
+  </si>
+  <si>
+    <t>Payment date</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>Optional note</t>
   </si>
 </sst>
 </file>
@@ -2121,6 +2233,300 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF2C7A8-C931-4428-947A-12DC12545B2D}">
+  <dimension ref="B2:E30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D519CBA-83CE-40E4-A866-C19D3BFF138A}">
   <dimension ref="B2:E24"/>
   <sheetViews>
@@ -2387,7 +2793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6657BDC6-C219-4021-B733-681CC5606BA5}">
   <dimension ref="B2:E12"/>
   <sheetViews>
@@ -2537,11 +2943,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72F04D2-B53F-4934-820F-AB2DEC1E3D20}">
   <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -2774,7 +3180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63415ECA-2024-443E-8C3D-8DB83C879615}">
   <dimension ref="B2:E18"/>
   <sheetViews>
@@ -3343,7 +3749,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B37" s="16" t="s">
         <v>446</v>
       </c>
@@ -3464,11 +3870,311 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2645935E-455F-4F73-860B-4037BE01AFAA}">
+  <dimension ref="B2:D35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="14" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>494</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7715187B-0C1D-4AFA-8862-89A2CA8C80DF}">
   <dimension ref="B2:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3785,7 +4491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519C62C8-D469-4AF1-BB98-19F9561484C7}">
   <dimension ref="B2:E27"/>
   <sheetViews>
@@ -4031,7 +4737,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6A5700-9044-4FA8-BD4C-C77EBDF7DE5A}">
   <dimension ref="B2:E26"/>
   <sheetViews>
@@ -4306,7 +5012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F1F487-B680-4D75-BCA6-2A07722803FE}">
   <dimension ref="B2:E39"/>
   <sheetViews>
@@ -4716,7 +5422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707F125F-AF2D-4F36-8BEB-A9E633D0F6A2}">
   <dimension ref="B2:E28"/>
   <sheetViews>
@@ -5033,7 +5739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D54EECB-50CD-46D6-9BAF-2E06F090346D}">
   <dimension ref="B2:E35"/>
   <sheetViews>
@@ -5399,298 +6105,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF2C7A8-C931-4428-947A-12DC12545B2D}">
-  <dimension ref="B2:E30"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>339</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>